<commit_message>
added arguments scope in cfc
</commit_message>
<xml_diff>
--- a/uploads/Upload_Result.xlsx
+++ b/uploads/Upload_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="32">
   <si>
     <t/>
   </si>
@@ -101,34 +101,13 @@
     <t>jaist@testmail.com</t>
   </si>
   <si>
-    <t>Jack</t>
-  </si>
-  <si>
-    <t>kottayam</t>
-  </si>
-  <si>
-    <t>ramika@testmail.com</t>
-  </si>
-  <si>
-    <t>Phone is missing</t>
-  </si>
-  <si>
-    <t>Jaiden</t>
-  </si>
-  <si>
-    <t>MB</t>
-  </si>
-  <si>
-    <t>Coimbatore</t>
-  </si>
-  <si>
-    <t>jaiden@testmail.com</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Role is not valid</t>
+    <t xml:space="preserve">James </t>
+  </si>
+  <si>
+    <t>Joy</t>
+  </si>
+  <si>
+    <t>Duplicate email entry found,Role is not valid</t>
   </si>
 </sst>
 </file>
@@ -191,7 +170,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -204,7 +183,7 @@
     <col min="5" max="5" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.15625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.91015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="25.984375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="40.61328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -391,54 +370,28 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="E8" t="n">
+        <v>7.89456123E9</v>
       </c>
       <c r="F8" t="n" s="2">
         <v>33101.0</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" t="n">
-        <v>7.8945625E8</v>
-      </c>
-      <c r="F9" t="n" s="2">
-        <v>33101.0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated update for duplicate email
</commit_message>
<xml_diff>
--- a/uploads/Upload_Result.xlsx
+++ b/uploads/Upload_Result.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="31">
   <si>
     <t/>
   </si>
@@ -56,7 +56,7 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>Duplicate email entry found</t>
+    <t>success</t>
   </si>
   <si>
     <t>Ram</t>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>Joy</t>
-  </si>
-  <si>
-    <t>Duplicate email entry found,Role is not valid</t>
   </si>
 </sst>
 </file>
@@ -183,7 +180,7 @@
     <col min="5" max="5" width="12.1875" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="12.15625" customWidth="true" bestFit="true"/>
     <col min="7" max="7" width="13.91015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="40.61328125" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="7.73046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -388,10 +385,10 @@
         <v>33101.0</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H8" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>